<commit_message>
#V1.0 fix# find some mistakes in signal-list and notes on schmatics. So modify it.
</commit_message>
<xml_diff>
--- a/XSS_MiniFOC_V1/Signal_List.xlsx
+++ b/XSS_MiniFOC_V1/Signal_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\EDA\Altium\XSS_MiniFOC_V1\XSS_MiniFOC_V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4F4A59-F1DE-46C5-9EE1-C1C243BCC1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E94796-F8BD-4994-BCD7-FE7FDC5FA474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -334,10 +334,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PB4/SPI2_MISO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SPI从机片选</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -426,14 +422,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PD1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PD2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MC_CHC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -467,6 +455,18 @@
   </si>
   <si>
     <t>PB4/SPI1_MISO(备用)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB6/SPI2_MISO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -574,6 +574,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -586,13 +593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -876,7 +876,7 @@
   <dimension ref="B2:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -906,10 +906,10 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>59</v>
@@ -917,13 +917,13 @@
       <c r="E3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -934,11 +934,11 @@
       <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -949,7 +949,7 @@
       <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
@@ -959,7 +959,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>34</v>
@@ -998,7 +998,7 @@
       <c r="E8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1015,7 +1015,7 @@
       <c r="E9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -1030,7 +1030,7 @@
       <c r="E10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
@@ -1070,7 +1070,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>36</v>
@@ -1092,7 +1092,7 @@
       <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1104,12 +1104,12 @@
         <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
@@ -1138,10 +1138,10 @@
       <c r="D20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="7" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1155,30 +1155,30 @@
       <c r="D21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="5"/>
+      <c r="D22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="6"/>
+        <v>107</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
@@ -1208,9 +1208,9 @@
         <v>70</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1222,12 +1222,12 @@
         <v>73</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="F29" s="8"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
@@ -1237,12 +1237,12 @@
         <v>74</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>80</v>
+      </c>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
@@ -1252,12 +1252,12 @@
         <v>75</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F31" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="F31" s="9"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
@@ -1284,7 +1284,7 @@
         <v>55</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>33</v>
@@ -1301,7 +1301,7 @@
         <v>56</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>33</v>
@@ -1315,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>2</v>
@@ -1329,74 +1329,74 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="F43" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="F20:F23"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="F3:F5"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="E20:E23"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="F20:F23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>